<commit_message>
修改HomeworkAppAction, FileAppAction, ClassAppAction 中AsycTask的执行
</commit_message>
<xml_diff>
--- a/基于Android的智慧移动课堂学习系统/App测试bug记录.xlsx
+++ b/基于Android的智慧移动课堂学习系统/App测试bug记录.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{4408D59B-CCF6-4AC6-AB23-1D46D7A4F0F1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{28273405-4E89-447F-AAF0-DF8D2E97B894}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
   <si>
     <t>代延绪</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -223,6 +223,10 @@
   </si>
   <si>
     <t>18.version.json返回的字符编码有问题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>已解决</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -556,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -780,17 +784,20 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>50</v>
       </c>

</xml_diff>

<commit_message>
修改InformAppAction, MaterialAppAction中AsycTask的执行 更新App测试记录 修复ListView头像乱显示bug 修复红点里显示数字bug 修复version.json乱码bug
</commit_message>
<xml_diff>
--- a/基于Android的智慧移动课堂学习系统/App测试bug记录.xlsx
+++ b/基于Android的智慧移动课堂学习系统/App测试bug记录.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{28273405-4E89-447F-AAF0-DF8D2E97B894}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{8EC6E41E-81DA-4B3A-838E-F475C675A472}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="59">
   <si>
     <t>代延绪</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -227,6 +227,34 @@
   </si>
   <si>
     <t>已解决</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>已解決</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16.作业名太长会导致经验值明细界面文字重叠</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>17.姓名改成maxLength="5"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>19.使用默认头像的用户刷新用户界面会一直刷新不结束</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>18.班课详情头像尽量少占用空间，右边第三行的数据显示不开，第三行三个字段的间隙也减少些</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15.班课成员太多，成员ListView 加载会头像错乱</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -560,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -602,6 +630,9 @@
       <c r="E2" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="F2" s="2" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -664,14 +695,23 @@
       <c r="C6" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="D6" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="E6" s="2" t="s">
         <v>32</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="B7" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="C7" s="2" t="s">
         <v>20</v>
       </c>
@@ -726,8 +766,14 @@
       <c r="C10" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="D10" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="E10" s="2" t="s">
         <v>47</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -751,6 +797,9 @@
       <c r="C12" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="D12" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -767,6 +816,9 @@
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="B14" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="C14" s="2" t="s">
         <v>41</v>
       </c>
@@ -778,28 +830,49 @@
       <c r="B15" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="C15" s="2" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>50</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>